<commit_message>
lookup broker SSI built
</commit_message>
<xml_diff>
--- a/reference/BLP_trade_sample2.xlsx
+++ b/reference/BLP_trade_sample2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\40019 trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E936698-8A3D-4EAA-A92C-C9ED215AA3C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010B7B44-9DCF-4714-B5E5-161E72D5FCD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="915" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="t9208529" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>China Life Franklin</t>
   </si>
@@ -128,12 +128,6 @@
   </si>
   <si>
     <t>B</t>
-  </si>
-  <si>
-    <t>15/10/20</t>
-  </si>
-  <si>
-    <t>21/10/20</t>
   </si>
   <si>
     <t>CHINA CITIC BANK INTERNATIONAL</t>
@@ -1117,13 +1111,13 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1193,7 +1187,7 @@
         <v>19</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -1252,12 +1246,12 @@
         <v>281310</v>
       </c>
       <c r="S4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" t="s">
-        <v>20</v>
+      <c r="A5">
+        <v>40019</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -1311,7 +1305,7 @@
         <v>281305</v>
       </c>
       <c r="S5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -1333,11 +1327,11 @@
       <c r="G6">
         <v>6.1234500000000001</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>37</v>
+      <c r="H6" s="1">
+        <v>44119</v>
+      </c>
+      <c r="I6" s="1">
+        <v>44125</v>
       </c>
       <c r="J6" s="3">
         <v>1379000</v>
@@ -1352,7 +1346,7 @@
         <v>25</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="O6" s="3">
         <v>0</v>
@@ -1367,7 +1361,7 @@
         <v>282617</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -1392,11 +1386,11 @@
       <c r="G7">
         <v>5.5549999999999997</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>37</v>
+      <c r="H7" s="1">
+        <v>44119</v>
+      </c>
+      <c r="I7" s="1">
+        <v>44125</v>
       </c>
       <c r="J7" s="3">
         <v>5000000</v>
@@ -1411,7 +1405,7 @@
         <v>25</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O7" s="3">
         <v>5833.33</v>
@@ -1426,7 +1420,7 @@
         <v>283003</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>